<commit_message>
First crack at the reboot
</commit_message>
<xml_diff>
--- a/tests/testthat/test_files/test_mkm_read.xlsx
+++ b/tests/testthat/test_files/test_mkm_read.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/mkm/tests/testthat/test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/Code/mkm/mkm/tests/testthat/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060B2E66-70B0-2D47-9058-F62B6FA57DC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDE032A-8F29-AD48-979A-AD091FDA5144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="37540" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transect" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>takiwaR Metadata</t>
   </si>
@@ -84,6 +92,9 @@
   </si>
   <si>
     <t>Substrate (% Cover)</t>
+  </si>
+  <si>
+    <t>empty section</t>
   </si>
 </sst>
 </file>
@@ -673,7 +684,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -836,7 +847,9 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="9"/>
+      <c r="A20" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2"/>

</xml_diff>